<commit_message>
added more of Joseline's screens, updated gui screens list
</commit_message>
<xml_diff>
--- a/GUI_Screens_List.xlsx
+++ b/GUI_Screens_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Desktop\UH Spring 2020\CIS 3365\Irina-Ya\AmberClad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2D83333-70A6-4D77-98BC-E6D4948FC30A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805F1DBA-A2D6-4B26-B794-94288110EBB4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38475" yWindow="525" windowWidth="15540" windowHeight="14610" xr2:uid="{9EDF0C0E-92AC-477D-978C-BFC2A7024A7D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9EDF0C0E-92AC-477D-978C-BFC2A7024A7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>GUI Screen</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Edit Bike</t>
   </si>
   <si>
-    <t>New Bike Manufacturer</t>
-  </si>
-  <si>
     <t>Edit Bike Manufacturer</t>
   </si>
   <si>
@@ -199,6 +196,12 @@
   </si>
   <si>
     <t>exhaustive menu of all repair order-related options</t>
+  </si>
+  <si>
+    <t>newBikeManufacturer</t>
+  </si>
+  <si>
+    <t>need to adjust - remove table just text fields/labels</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -652,7 +655,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -673,7 +676,7 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -681,7 +684,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -729,7 +732,7 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -745,7 +748,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -753,7 +756,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -765,19 +768,25 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -809,8 +818,11 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -818,59 +830,65 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>